<commit_message>
Add manual raw data.
Add 2018 CRBA results for validation.

Update sdmx value mapping.
</commit_message>
<xml_diff>
--- a/data_in/data_raw_manually_extracted/human_entered/S_233.xlsx
+++ b/data_in/data_raw_manually_extracted/human_entered/S_233.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11108"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pixie/Desktop/Data meeting/Data collection/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://unicef.sharepoint.com/teams/CHE-MarketData-DataIngest/Shared Documents/Data Ingest/CRB Atlas/data_raw_manually_extracted/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A357C17-0ED4-584A-8FB9-4EA9050D99F3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="6" documentId="13_ncr:1_{8A357C17-0ED4-584A-8FB9-4EA9050D99F3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{1BE5722A-56ED-4DFE-8565-195762580DA6}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="19780" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="23880" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Blueprint" sheetId="1" r:id="rId1"/>
@@ -22,6 +22,7 @@
     <externalReference r:id="rId5"/>
   </externalReferences>
   <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Blueprint!$A$1:$AJ$196</definedName>
     <definedName name="Options_2.3Sb">[1]CRCE!$DQ$212:$DQ$219</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
@@ -2398,39 +2399,40 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:AJ196"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="T191" sqref="T191"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="2" width="15.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="15.44140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="16" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.1640625" customWidth="1"/>
-    <col min="5" max="5" width="17.5" customWidth="1"/>
-    <col min="7" max="7" width="15.1640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.1640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="16.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.109375" customWidth="1"/>
+    <col min="5" max="5" width="17.44140625" customWidth="1"/>
+    <col min="7" max="7" width="15.109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.77734375" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="15.33203125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="20" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="14" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="25.1640625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="12.1640625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="14.5" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="25.109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="12.109375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="14.44140625" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="14.6640625" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="25.6640625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="20.1640625" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="19.1640625" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="29.83203125" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="24.83203125" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="22.83203125" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="25.83203125" customWidth="1"/>
+    <col min="18" max="18" width="20.109375" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="19.109375" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="29.77734375" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="24.77734375" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="22.77734375" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="25.77734375" customWidth="1"/>
     <col min="24" max="24" width="24.6640625" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="27.1640625" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="19.1640625" customWidth="1"/>
-    <col min="27" max="27" width="8.83203125" customWidth="1"/>
+    <col min="25" max="25" width="27.109375" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="19.109375" customWidth="1"/>
+    <col min="27" max="27" width="8.77734375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:36" s="1" customFormat="1">
@@ -2538,7 +2540,7 @@
       </c>
       <c r="AJ1" s="5"/>
     </row>
-    <row r="2" spans="1:36" ht="16">
+    <row r="2" spans="1:36" ht="15.6" hidden="1">
       <c r="A2" s="7" t="s">
         <v>24</v>
       </c>
@@ -2589,7 +2591,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="3" spans="1:36" ht="16">
+    <row r="3" spans="1:36" ht="15.6" hidden="1">
       <c r="A3" s="7" t="s">
         <v>85</v>
       </c>
@@ -2608,7 +2610,7 @@
       </c>
       <c r="Z3" s="3"/>
     </row>
-    <row r="4" spans="1:36" ht="16">
+    <row r="4" spans="1:36" ht="15.6" hidden="1">
       <c r="A4" s="7" t="s">
         <v>89</v>
       </c>
@@ -2626,7 +2628,7 @@
         <v>573</v>
       </c>
     </row>
-    <row r="5" spans="1:36" ht="16">
+    <row r="5" spans="1:36" ht="15.6" hidden="1">
       <c r="A5" s="7" t="s">
         <v>90</v>
       </c>
@@ -2644,7 +2646,7 @@
         <v>573</v>
       </c>
     </row>
-    <row r="6" spans="1:36" ht="16">
+    <row r="6" spans="1:36" ht="15.6" hidden="1">
       <c r="A6" s="7" t="s">
         <v>91</v>
       </c>
@@ -2662,7 +2664,7 @@
         <v>573</v>
       </c>
     </row>
-    <row r="7" spans="1:36" ht="16">
+    <row r="7" spans="1:36" ht="15.6" hidden="1">
       <c r="A7" s="7" t="s">
         <v>2</v>
       </c>
@@ -2680,7 +2682,7 @@
         <v>573</v>
       </c>
     </row>
-    <row r="8" spans="1:36" ht="16">
+    <row r="8" spans="1:36" ht="15.6" hidden="1">
       <c r="A8" s="7" t="s">
         <v>1</v>
       </c>
@@ -2698,7 +2700,7 @@
         <v>573</v>
       </c>
     </row>
-    <row r="9" spans="1:36" ht="16">
+    <row r="9" spans="1:36" ht="15.6" hidden="1">
       <c r="A9" s="7" t="s">
         <v>92</v>
       </c>
@@ -2716,7 +2718,7 @@
         <v>573</v>
       </c>
     </row>
-    <row r="10" spans="1:36" ht="16">
+    <row r="10" spans="1:36" ht="15.6" hidden="1">
       <c r="A10" s="7" t="s">
         <v>93</v>
       </c>
@@ -2734,7 +2736,7 @@
         <v>573</v>
       </c>
     </row>
-    <row r="11" spans="1:36" ht="16">
+    <row r="11" spans="1:36" ht="15.6" hidden="1">
       <c r="A11" s="7" t="s">
         <v>94</v>
       </c>
@@ -2752,7 +2754,7 @@
         <v>573</v>
       </c>
     </row>
-    <row r="12" spans="1:36" ht="16">
+    <row r="12" spans="1:36" ht="15.6" hidden="1">
       <c r="A12" s="7" t="s">
         <v>95</v>
       </c>
@@ -2770,7 +2772,7 @@
         <v>573</v>
       </c>
     </row>
-    <row r="13" spans="1:36" ht="16">
+    <row r="13" spans="1:36" ht="15.6" hidden="1">
       <c r="A13" s="7" t="s">
         <v>96</v>
       </c>
@@ -2788,7 +2790,7 @@
         <v>573</v>
       </c>
     </row>
-    <row r="14" spans="1:36" ht="16">
+    <row r="14" spans="1:36" ht="15.6" hidden="1">
       <c r="A14" s="7" t="s">
         <v>97</v>
       </c>
@@ -2806,7 +2808,7 @@
         <v>573</v>
       </c>
     </row>
-    <row r="15" spans="1:36" ht="16">
+    <row r="15" spans="1:36" ht="15.6" hidden="1">
       <c r="A15" s="7" t="s">
         <v>98</v>
       </c>
@@ -2824,7 +2826,7 @@
         <v>573</v>
       </c>
     </row>
-    <row r="16" spans="1:36" ht="16">
+    <row r="16" spans="1:36" ht="15.6" hidden="1">
       <c r="A16" s="7" t="s">
         <v>99</v>
       </c>
@@ -2842,7 +2844,7 @@
         <v>573</v>
       </c>
     </row>
-    <row r="17" spans="1:20" ht="16">
+    <row r="17" spans="1:20" ht="15.6" hidden="1">
       <c r="A17" s="7" t="s">
         <v>100</v>
       </c>
@@ -2860,7 +2862,7 @@
         <v>573</v>
       </c>
     </row>
-    <row r="18" spans="1:20" ht="16">
+    <row r="18" spans="1:20" ht="15.6" hidden="1">
       <c r="A18" s="7" t="s">
         <v>101</v>
       </c>
@@ -2878,7 +2880,7 @@
         <v>573</v>
       </c>
     </row>
-    <row r="19" spans="1:20" ht="16">
+    <row r="19" spans="1:20" ht="15.6" hidden="1">
       <c r="A19" s="7" t="s">
         <v>102</v>
       </c>
@@ -2896,7 +2898,7 @@
         <v>573</v>
       </c>
     </row>
-    <row r="20" spans="1:20" ht="16">
+    <row r="20" spans="1:20" ht="15.6" hidden="1">
       <c r="A20" s="7" t="s">
         <v>103</v>
       </c>
@@ -2914,7 +2916,7 @@
         <v>573</v>
       </c>
     </row>
-    <row r="21" spans="1:20" ht="16">
+    <row r="21" spans="1:20" ht="15.6" hidden="1">
       <c r="A21" s="7" t="s">
         <v>104</v>
       </c>
@@ -2932,7 +2934,7 @@
         <v>573</v>
       </c>
     </row>
-    <row r="22" spans="1:20" ht="16">
+    <row r="22" spans="1:20" ht="15.6" hidden="1">
       <c r="A22" s="7" t="s">
         <v>105</v>
       </c>
@@ -2950,7 +2952,7 @@
         <v>573</v>
       </c>
     </row>
-    <row r="23" spans="1:20" ht="16">
+    <row r="23" spans="1:20" ht="15.6" hidden="1">
       <c r="A23" s="7" t="s">
         <v>106</v>
       </c>
@@ -2968,7 +2970,7 @@
         <v>573</v>
       </c>
     </row>
-    <row r="24" spans="1:20" ht="16">
+    <row r="24" spans="1:20" ht="15.6" hidden="1">
       <c r="A24" s="7" t="s">
         <v>107</v>
       </c>
@@ -2986,7 +2988,7 @@
         <v>573</v>
       </c>
     </row>
-    <row r="25" spans="1:20" ht="16">
+    <row r="25" spans="1:20" ht="15.6" hidden="1">
       <c r="A25" s="7" t="s">
         <v>108</v>
       </c>
@@ -3004,7 +3006,7 @@
         <v>573</v>
       </c>
     </row>
-    <row r="26" spans="1:20" ht="16">
+    <row r="26" spans="1:20" ht="15.6" hidden="1">
       <c r="A26" s="7" t="s">
         <v>109</v>
       </c>
@@ -3022,7 +3024,7 @@
         <v>573</v>
       </c>
     </row>
-    <row r="27" spans="1:20" ht="16">
+    <row r="27" spans="1:20" ht="15.6" hidden="1">
       <c r="A27" s="7" t="s">
         <v>110</v>
       </c>
@@ -3040,7 +3042,7 @@
         <v>573</v>
       </c>
     </row>
-    <row r="28" spans="1:20" ht="16">
+    <row r="28" spans="1:20" ht="15.6">
       <c r="A28" s="7" t="s">
         <v>111</v>
       </c>
@@ -3058,7 +3060,7 @@
         <v>573</v>
       </c>
     </row>
-    <row r="29" spans="1:20" ht="16">
+    <row r="29" spans="1:20" ht="15.6" hidden="1">
       <c r="A29" s="7" t="s">
         <v>112</v>
       </c>
@@ -3076,7 +3078,7 @@
         <v>573</v>
       </c>
     </row>
-    <row r="30" spans="1:20" ht="16">
+    <row r="30" spans="1:20" ht="15.6" hidden="1">
       <c r="A30" s="7" t="s">
         <v>113</v>
       </c>
@@ -3094,7 +3096,7 @@
         <v>573</v>
       </c>
     </row>
-    <row r="31" spans="1:20" ht="16">
+    <row r="31" spans="1:20" ht="15.6" hidden="1">
       <c r="A31" s="7" t="s">
         <v>114</v>
       </c>
@@ -3112,7 +3114,7 @@
         <v>573</v>
       </c>
     </row>
-    <row r="32" spans="1:20" ht="16">
+    <row r="32" spans="1:20" ht="15.6" hidden="1">
       <c r="A32" s="7" t="s">
         <v>115</v>
       </c>
@@ -3130,7 +3132,7 @@
         <v>573</v>
       </c>
     </row>
-    <row r="33" spans="1:20" ht="16">
+    <row r="33" spans="1:20" ht="15.6" hidden="1">
       <c r="A33" s="7" t="s">
         <v>116</v>
       </c>
@@ -3148,7 +3150,7 @@
         <v>573</v>
       </c>
     </row>
-    <row r="34" spans="1:20" ht="16">
+    <row r="34" spans="1:20" ht="15.6" hidden="1">
       <c r="A34" s="7" t="s">
         <v>117</v>
       </c>
@@ -3166,7 +3168,7 @@
         <v>573</v>
       </c>
     </row>
-    <row r="35" spans="1:20" ht="16">
+    <row r="35" spans="1:20" ht="15.6" hidden="1">
       <c r="A35" s="7" t="s">
         <v>118</v>
       </c>
@@ -3184,7 +3186,7 @@
         <v>573</v>
       </c>
     </row>
-    <row r="36" spans="1:20" ht="16">
+    <row r="36" spans="1:20" ht="15.6" hidden="1">
       <c r="A36" s="7" t="s">
         <v>119</v>
       </c>
@@ -3202,7 +3204,7 @@
         <v>573</v>
       </c>
     </row>
-    <row r="37" spans="1:20" ht="16">
+    <row r="37" spans="1:20" ht="15.6">
       <c r="A37" s="7" t="s">
         <v>120</v>
       </c>
@@ -3220,7 +3222,7 @@
         <v>573</v>
       </c>
     </row>
-    <row r="38" spans="1:20" ht="16">
+    <row r="38" spans="1:20" ht="15.6">
       <c r="A38" s="7" t="s">
         <v>121</v>
       </c>
@@ -3238,7 +3240,7 @@
         <v>573</v>
       </c>
     </row>
-    <row r="39" spans="1:20" ht="16">
+    <row r="39" spans="1:20" ht="15.6" hidden="1">
       <c r="A39" s="7" t="s">
         <v>122</v>
       </c>
@@ -3256,7 +3258,7 @@
         <v>573</v>
       </c>
     </row>
-    <row r="40" spans="1:20" ht="16">
+    <row r="40" spans="1:20" ht="15.6" hidden="1">
       <c r="A40" s="7" t="s">
         <v>123</v>
       </c>
@@ -3274,7 +3276,7 @@
         <v>573</v>
       </c>
     </row>
-    <row r="41" spans="1:20" ht="16">
+    <row r="41" spans="1:20" ht="15.6" hidden="1">
       <c r="A41" s="7" t="s">
         <v>124</v>
       </c>
@@ -3292,7 +3294,7 @@
         <v>573</v>
       </c>
     </row>
-    <row r="42" spans="1:20" ht="16">
+    <row r="42" spans="1:20" ht="15.6" hidden="1">
       <c r="A42" s="7" t="s">
         <v>125</v>
       </c>
@@ -3310,7 +3312,7 @@
         <v>573</v>
       </c>
     </row>
-    <row r="43" spans="1:20" ht="16">
+    <row r="43" spans="1:20" ht="15.6" hidden="1">
       <c r="A43" s="7" t="s">
         <v>126</v>
       </c>
@@ -3328,7 +3330,7 @@
         <v>573</v>
       </c>
     </row>
-    <row r="44" spans="1:20" ht="16">
+    <row r="44" spans="1:20" ht="15.6" hidden="1">
       <c r="A44" s="7" t="s">
         <v>127</v>
       </c>
@@ -3346,7 +3348,7 @@
         <v>573</v>
       </c>
     </row>
-    <row r="45" spans="1:20" ht="16">
+    <row r="45" spans="1:20" ht="15.6" hidden="1">
       <c r="A45" s="7" t="s">
         <v>128</v>
       </c>
@@ -3364,7 +3366,7 @@
         <v>573</v>
       </c>
     </row>
-    <row r="46" spans="1:20" ht="16">
+    <row r="46" spans="1:20" ht="15.6" hidden="1">
       <c r="A46" s="7" t="s">
         <v>129</v>
       </c>
@@ -3382,7 +3384,7 @@
         <v>573</v>
       </c>
     </row>
-    <row r="47" spans="1:20" ht="16">
+    <row r="47" spans="1:20" ht="15.6" hidden="1">
       <c r="A47" s="7" t="s">
         <v>130</v>
       </c>
@@ -3400,7 +3402,7 @@
         <v>573</v>
       </c>
     </row>
-    <row r="48" spans="1:20" ht="16">
+    <row r="48" spans="1:20" ht="15.6" hidden="1">
       <c r="A48" s="7" t="s">
         <v>131</v>
       </c>
@@ -3418,7 +3420,7 @@
         <v>573</v>
       </c>
     </row>
-    <row r="49" spans="1:20" ht="16">
+    <row r="49" spans="1:20" ht="15.6" hidden="1">
       <c r="A49" s="7" t="s">
         <v>132</v>
       </c>
@@ -3436,7 +3438,7 @@
         <v>573</v>
       </c>
     </row>
-    <row r="50" spans="1:20" ht="16">
+    <row r="50" spans="1:20" ht="15.6" hidden="1">
       <c r="A50" s="7" t="s">
         <v>133</v>
       </c>
@@ -3454,7 +3456,7 @@
         <v>573</v>
       </c>
     </row>
-    <row r="51" spans="1:20" ht="16">
+    <row r="51" spans="1:20" ht="15.6" hidden="1">
       <c r="A51" s="7" t="s">
         <v>134</v>
       </c>
@@ -3472,7 +3474,7 @@
         <v>573</v>
       </c>
     </row>
-    <row r="52" spans="1:20" ht="16">
+    <row r="52" spans="1:20" ht="15.6">
       <c r="A52" s="7" t="s">
         <v>135</v>
       </c>
@@ -3490,7 +3492,7 @@
         <v>573</v>
       </c>
     </row>
-    <row r="53" spans="1:20" ht="16">
+    <row r="53" spans="1:20" ht="15.6" hidden="1">
       <c r="A53" s="7" t="s">
         <v>136</v>
       </c>
@@ -3508,7 +3510,7 @@
         <v>573</v>
       </c>
     </row>
-    <row r="54" spans="1:20" ht="16">
+    <row r="54" spans="1:20" ht="15.6" hidden="1">
       <c r="A54" s="7" t="s">
         <v>137</v>
       </c>
@@ -3526,7 +3528,7 @@
         <v>573</v>
       </c>
     </row>
-    <row r="55" spans="1:20" ht="16">
+    <row r="55" spans="1:20" ht="15.6" hidden="1">
       <c r="A55" s="7" t="s">
         <v>138</v>
       </c>
@@ -3544,7 +3546,7 @@
         <v>573</v>
       </c>
     </row>
-    <row r="56" spans="1:20" ht="16">
+    <row r="56" spans="1:20" ht="15.6" hidden="1">
       <c r="A56" s="7" t="s">
         <v>139</v>
       </c>
@@ -3562,7 +3564,7 @@
         <v>573</v>
       </c>
     </row>
-    <row r="57" spans="1:20" ht="16">
+    <row r="57" spans="1:20" ht="15.6" hidden="1">
       <c r="A57" s="7" t="s">
         <v>140</v>
       </c>
@@ -3580,7 +3582,7 @@
         <v>573</v>
       </c>
     </row>
-    <row r="58" spans="1:20" ht="16">
+    <row r="58" spans="1:20" ht="15.6" hidden="1">
       <c r="A58" s="7" t="s">
         <v>141</v>
       </c>
@@ -3598,7 +3600,7 @@
         <v>573</v>
       </c>
     </row>
-    <row r="59" spans="1:20" ht="16">
+    <row r="59" spans="1:20" ht="15.6" hidden="1">
       <c r="A59" s="7" t="s">
         <v>142</v>
       </c>
@@ -3616,7 +3618,7 @@
         <v>573</v>
       </c>
     </row>
-    <row r="60" spans="1:20" ht="16">
+    <row r="60" spans="1:20" ht="15.6" hidden="1">
       <c r="A60" s="7" t="s">
         <v>143</v>
       </c>
@@ -3634,7 +3636,7 @@
         <v>573</v>
       </c>
     </row>
-    <row r="61" spans="1:20" ht="16">
+    <row r="61" spans="1:20" ht="15.6" hidden="1">
       <c r="A61" s="7" t="s">
         <v>144</v>
       </c>
@@ -3652,7 +3654,7 @@
         <v>573</v>
       </c>
     </row>
-    <row r="62" spans="1:20" ht="16">
+    <row r="62" spans="1:20" ht="15.6" hidden="1">
       <c r="A62" s="7" t="s">
         <v>145</v>
       </c>
@@ -3670,7 +3672,7 @@
         <v>573</v>
       </c>
     </row>
-    <row r="63" spans="1:20" ht="16">
+    <row r="63" spans="1:20" ht="15.6" hidden="1">
       <c r="A63" s="7" t="s">
         <v>146</v>
       </c>
@@ -3688,7 +3690,7 @@
         <v>573</v>
       </c>
     </row>
-    <row r="64" spans="1:20" ht="16">
+    <row r="64" spans="1:20" ht="15.6" hidden="1">
       <c r="A64" s="7" t="s">
         <v>147</v>
       </c>
@@ -3706,7 +3708,7 @@
         <v>573</v>
       </c>
     </row>
-    <row r="65" spans="1:20" ht="16">
+    <row r="65" spans="1:20" ht="15.6" hidden="1">
       <c r="A65" s="7" t="s">
         <v>148</v>
       </c>
@@ -3724,7 +3726,7 @@
         <v>573</v>
       </c>
     </row>
-    <row r="66" spans="1:20" ht="16">
+    <row r="66" spans="1:20" ht="15.6" hidden="1">
       <c r="A66" s="7" t="s">
         <v>149</v>
       </c>
@@ -3742,7 +3744,7 @@
         <v>573</v>
       </c>
     </row>
-    <row r="67" spans="1:20" ht="16">
+    <row r="67" spans="1:20" ht="15.6">
       <c r="A67" s="7" t="s">
         <v>150</v>
       </c>
@@ -3753,14 +3755,14 @@
         <v>2019</v>
       </c>
       <c r="E67" t="s">
-        <v>572</v>
+        <v>575</v>
       </c>
       <c r="S67" s="6"/>
       <c r="T67" s="27" t="s">
         <v>573</v>
       </c>
     </row>
-    <row r="68" spans="1:20" ht="16">
+    <row r="68" spans="1:20" ht="15.6" hidden="1">
       <c r="A68" s="7" t="s">
         <v>151</v>
       </c>
@@ -3778,7 +3780,7 @@
         <v>573</v>
       </c>
     </row>
-    <row r="69" spans="1:20" ht="16">
+    <row r="69" spans="1:20" ht="15.6" hidden="1">
       <c r="A69" s="7" t="s">
         <v>152</v>
       </c>
@@ -3796,7 +3798,7 @@
         <v>573</v>
       </c>
     </row>
-    <row r="70" spans="1:20" ht="16">
+    <row r="70" spans="1:20" ht="15.6" hidden="1">
       <c r="A70" s="7" t="s">
         <v>153</v>
       </c>
@@ -3814,7 +3816,7 @@
         <v>573</v>
       </c>
     </row>
-    <row r="71" spans="1:20" ht="16">
+    <row r="71" spans="1:20" ht="15.6" hidden="1">
       <c r="A71" s="7" t="s">
         <v>154</v>
       </c>
@@ -3832,7 +3834,7 @@
         <v>573</v>
       </c>
     </row>
-    <row r="72" spans="1:20" ht="16">
+    <row r="72" spans="1:20" ht="15.6" hidden="1">
       <c r="A72" s="7" t="s">
         <v>155</v>
       </c>
@@ -3850,7 +3852,7 @@
         <v>573</v>
       </c>
     </row>
-    <row r="73" spans="1:20" ht="16">
+    <row r="73" spans="1:20" ht="15.6" hidden="1">
       <c r="A73" s="7" t="s">
         <v>156</v>
       </c>
@@ -3868,7 +3870,7 @@
         <v>573</v>
       </c>
     </row>
-    <row r="74" spans="1:20" ht="16">
+    <row r="74" spans="1:20" ht="15.6" hidden="1">
       <c r="A74" s="7" t="s">
         <v>157</v>
       </c>
@@ -3886,7 +3888,7 @@
         <v>573</v>
       </c>
     </row>
-    <row r="75" spans="1:20" ht="16">
+    <row r="75" spans="1:20" ht="15.6" hidden="1">
       <c r="A75" s="7" t="s">
         <v>158</v>
       </c>
@@ -3904,7 +3906,7 @@
         <v>573</v>
       </c>
     </row>
-    <row r="76" spans="1:20" ht="16">
+    <row r="76" spans="1:20" ht="15.6" hidden="1">
       <c r="A76" s="7" t="s">
         <v>159</v>
       </c>
@@ -3922,7 +3924,7 @@
         <v>573</v>
       </c>
     </row>
-    <row r="77" spans="1:20" ht="16">
+    <row r="77" spans="1:20" ht="15.6" hidden="1">
       <c r="A77" s="7" t="s">
         <v>160</v>
       </c>
@@ -3933,14 +3935,14 @@
         <v>2019</v>
       </c>
       <c r="E77" t="s">
-        <v>571</v>
+        <v>574</v>
       </c>
       <c r="S77" s="6"/>
       <c r="T77" s="27" t="s">
         <v>573</v>
       </c>
     </row>
-    <row r="78" spans="1:20" ht="16">
+    <row r="78" spans="1:20" ht="15.6" hidden="1">
       <c r="A78" s="7" t="s">
         <v>161</v>
       </c>
@@ -3958,7 +3960,7 @@
         <v>573</v>
       </c>
     </row>
-    <row r="79" spans="1:20" ht="16">
+    <row r="79" spans="1:20" ht="15.6" hidden="1">
       <c r="A79" s="7" t="s">
         <v>162</v>
       </c>
@@ -3976,7 +3978,7 @@
         <v>573</v>
       </c>
     </row>
-    <row r="80" spans="1:20" ht="16">
+    <row r="80" spans="1:20" ht="15.6" hidden="1">
       <c r="A80" s="7" t="s">
         <v>163</v>
       </c>
@@ -3994,7 +3996,7 @@
         <v>573</v>
       </c>
     </row>
-    <row r="81" spans="1:20" ht="16">
+    <row r="81" spans="1:20" ht="15.6" hidden="1">
       <c r="A81" s="7" t="s">
         <v>164</v>
       </c>
@@ -4012,7 +4014,7 @@
         <v>573</v>
       </c>
     </row>
-    <row r="82" spans="1:20" ht="16">
+    <row r="82" spans="1:20" ht="15.6" hidden="1">
       <c r="A82" s="7" t="s">
         <v>165</v>
       </c>
@@ -4030,7 +4032,7 @@
         <v>573</v>
       </c>
     </row>
-    <row r="83" spans="1:20" ht="16">
+    <row r="83" spans="1:20" ht="15.6" hidden="1">
       <c r="A83" s="7" t="s">
         <v>166</v>
       </c>
@@ -4048,7 +4050,7 @@
         <v>573</v>
       </c>
     </row>
-    <row r="84" spans="1:20" ht="16">
+    <row r="84" spans="1:20" ht="15.6" hidden="1">
       <c r="A84" s="7" t="s">
         <v>167</v>
       </c>
@@ -4066,7 +4068,7 @@
         <v>573</v>
       </c>
     </row>
-    <row r="85" spans="1:20" ht="16">
+    <row r="85" spans="1:20" ht="15.6" hidden="1">
       <c r="A85" s="7" t="s">
         <v>168</v>
       </c>
@@ -4084,7 +4086,7 @@
         <v>573</v>
       </c>
     </row>
-    <row r="86" spans="1:20" ht="16">
+    <row r="86" spans="1:20" ht="15.6" hidden="1">
       <c r="A86" s="7" t="s">
         <v>169</v>
       </c>
@@ -4102,7 +4104,7 @@
         <v>573</v>
       </c>
     </row>
-    <row r="87" spans="1:20" ht="16">
+    <row r="87" spans="1:20" ht="15.6" hidden="1">
       <c r="A87" s="7" t="s">
         <v>170</v>
       </c>
@@ -4120,7 +4122,7 @@
         <v>573</v>
       </c>
     </row>
-    <row r="88" spans="1:20" ht="16">
+    <row r="88" spans="1:20" ht="15.6" hidden="1">
       <c r="A88" s="7" t="s">
         <v>171</v>
       </c>
@@ -4138,7 +4140,7 @@
         <v>573</v>
       </c>
     </row>
-    <row r="89" spans="1:20" ht="16">
+    <row r="89" spans="1:20" ht="15.6">
       <c r="A89" s="7" t="s">
         <v>172</v>
       </c>
@@ -4156,7 +4158,7 @@
         <v>573</v>
       </c>
     </row>
-    <row r="90" spans="1:20" ht="16">
+    <row r="90" spans="1:20" ht="15.6" hidden="1">
       <c r="A90" s="7" t="s">
         <v>173</v>
       </c>
@@ -4174,7 +4176,7 @@
         <v>573</v>
       </c>
     </row>
-    <row r="91" spans="1:20" ht="16">
+    <row r="91" spans="1:20" ht="15.6" hidden="1">
       <c r="A91" s="7" t="s">
         <v>174</v>
       </c>
@@ -4192,7 +4194,7 @@
         <v>573</v>
       </c>
     </row>
-    <row r="92" spans="1:20" ht="16">
+    <row r="92" spans="1:20" ht="15.6" hidden="1">
       <c r="A92" s="7" t="s">
         <v>175</v>
       </c>
@@ -4210,7 +4212,7 @@
         <v>573</v>
       </c>
     </row>
-    <row r="93" spans="1:20" ht="16">
+    <row r="93" spans="1:20" ht="15.6" hidden="1">
       <c r="A93" s="7" t="s">
         <v>459</v>
       </c>
@@ -4228,7 +4230,7 @@
         <v>573</v>
       </c>
     </row>
-    <row r="94" spans="1:20" ht="16">
+    <row r="94" spans="1:20" ht="15.6" hidden="1">
       <c r="A94" s="7" t="s">
         <v>177</v>
       </c>
@@ -4246,7 +4248,7 @@
         <v>573</v>
       </c>
     </row>
-    <row r="95" spans="1:20" ht="16">
+    <row r="95" spans="1:20" ht="15.6" hidden="1">
       <c r="A95" s="7" t="s">
         <v>178</v>
       </c>
@@ -4264,7 +4266,7 @@
         <v>573</v>
       </c>
     </row>
-    <row r="96" spans="1:20" ht="16">
+    <row r="96" spans="1:20" ht="15.6" hidden="1">
       <c r="A96" s="7" t="s">
         <v>179</v>
       </c>
@@ -4282,7 +4284,7 @@
         <v>573</v>
       </c>
     </row>
-    <row r="97" spans="1:20" ht="16">
+    <row r="97" spans="1:20" ht="15.6" hidden="1">
       <c r="A97" s="7" t="s">
         <v>180</v>
       </c>
@@ -4300,7 +4302,7 @@
         <v>573</v>
       </c>
     </row>
-    <row r="98" spans="1:20" ht="16">
+    <row r="98" spans="1:20" ht="15.6" hidden="1">
       <c r="A98" s="7" t="s">
         <v>181</v>
       </c>
@@ -4318,7 +4320,7 @@
         <v>573</v>
       </c>
     </row>
-    <row r="99" spans="1:20" ht="16">
+    <row r="99" spans="1:20" ht="15.6" hidden="1">
       <c r="A99" s="7" t="s">
         <v>182</v>
       </c>
@@ -4336,7 +4338,7 @@
         <v>573</v>
       </c>
     </row>
-    <row r="100" spans="1:20" ht="16">
+    <row r="100" spans="1:20" ht="15.6" hidden="1">
       <c r="A100" s="7" t="s">
         <v>183</v>
       </c>
@@ -4354,7 +4356,7 @@
         <v>573</v>
       </c>
     </row>
-    <row r="101" spans="1:20" ht="16">
+    <row r="101" spans="1:20" ht="15.6" hidden="1">
       <c r="A101" s="7" t="s">
         <v>184</v>
       </c>
@@ -4372,7 +4374,7 @@
         <v>573</v>
       </c>
     </row>
-    <row r="102" spans="1:20" ht="16">
+    <row r="102" spans="1:20" ht="15.6" hidden="1">
       <c r="A102" s="7" t="s">
         <v>185</v>
       </c>
@@ -4390,7 +4392,7 @@
         <v>573</v>
       </c>
     </row>
-    <row r="103" spans="1:20" ht="16">
+    <row r="103" spans="1:20" ht="15.6" hidden="1">
       <c r="A103" s="7" t="s">
         <v>186</v>
       </c>
@@ -4408,7 +4410,7 @@
         <v>573</v>
       </c>
     </row>
-    <row r="104" spans="1:20" ht="16">
+    <row r="104" spans="1:20" ht="15.6" hidden="1">
       <c r="A104" s="7" t="s">
         <v>187</v>
       </c>
@@ -4426,7 +4428,7 @@
         <v>573</v>
       </c>
     </row>
-    <row r="105" spans="1:20" ht="16">
+    <row r="105" spans="1:20" ht="15.6" hidden="1">
       <c r="A105" s="7" t="s">
         <v>188</v>
       </c>
@@ -4444,7 +4446,7 @@
         <v>573</v>
       </c>
     </row>
-    <row r="106" spans="1:20" ht="16">
+    <row r="106" spans="1:20" ht="15.6" hidden="1">
       <c r="A106" s="7" t="s">
         <v>189</v>
       </c>
@@ -4462,7 +4464,7 @@
         <v>573</v>
       </c>
     </row>
-    <row r="107" spans="1:20" ht="16">
+    <row r="107" spans="1:20" ht="15.6" hidden="1">
       <c r="A107" s="7" t="s">
         <v>190</v>
       </c>
@@ -4480,7 +4482,7 @@
         <v>573</v>
       </c>
     </row>
-    <row r="108" spans="1:20" ht="16">
+    <row r="108" spans="1:20" ht="15.6" hidden="1">
       <c r="A108" s="7" t="s">
         <v>191</v>
       </c>
@@ -4498,7 +4500,7 @@
         <v>573</v>
       </c>
     </row>
-    <row r="109" spans="1:20" ht="16">
+    <row r="109" spans="1:20" ht="15.6" hidden="1">
       <c r="A109" s="7" t="s">
         <v>192</v>
       </c>
@@ -4516,7 +4518,7 @@
         <v>573</v>
       </c>
     </row>
-    <row r="110" spans="1:20" ht="16">
+    <row r="110" spans="1:20" ht="15.6" hidden="1">
       <c r="A110" s="7" t="s">
         <v>193</v>
       </c>
@@ -4534,7 +4536,7 @@
         <v>573</v>
       </c>
     </row>
-    <row r="111" spans="1:20" ht="16">
+    <row r="111" spans="1:20" ht="15.6" hidden="1">
       <c r="A111" s="7" t="s">
         <v>194</v>
       </c>
@@ -4552,7 +4554,7 @@
         <v>573</v>
       </c>
     </row>
-    <row r="112" spans="1:20" ht="16">
+    <row r="112" spans="1:20" ht="15.6" hidden="1">
       <c r="A112" s="7" t="s">
         <v>195</v>
       </c>
@@ -4570,7 +4572,7 @@
         <v>573</v>
       </c>
     </row>
-    <row r="113" spans="1:20" ht="16">
+    <row r="113" spans="1:20" ht="15.6" hidden="1">
       <c r="A113" s="7" t="s">
         <v>196</v>
       </c>
@@ -4588,7 +4590,7 @@
         <v>573</v>
       </c>
     </row>
-    <row r="114" spans="1:20" ht="16">
+    <row r="114" spans="1:20" ht="15.6" hidden="1">
       <c r="A114" s="7" t="s">
         <v>197</v>
       </c>
@@ -4606,7 +4608,7 @@
         <v>573</v>
       </c>
     </row>
-    <row r="115" spans="1:20" ht="16">
+    <row r="115" spans="1:20" ht="15.6" hidden="1">
       <c r="A115" s="7" t="s">
         <v>198</v>
       </c>
@@ -4624,7 +4626,7 @@
         <v>573</v>
       </c>
     </row>
-    <row r="116" spans="1:20" ht="16">
+    <row r="116" spans="1:20" ht="15.6" hidden="1">
       <c r="A116" s="7" t="s">
         <v>199</v>
       </c>
@@ -4642,7 +4644,7 @@
         <v>573</v>
       </c>
     </row>
-    <row r="117" spans="1:20" ht="16">
+    <row r="117" spans="1:20" ht="15.6" hidden="1">
       <c r="A117" s="7" t="s">
         <v>200</v>
       </c>
@@ -4660,7 +4662,7 @@
         <v>573</v>
       </c>
     </row>
-    <row r="118" spans="1:20" ht="16">
+    <row r="118" spans="1:20" ht="15.6" hidden="1">
       <c r="A118" s="7" t="s">
         <v>201</v>
       </c>
@@ -4678,7 +4680,7 @@
         <v>573</v>
       </c>
     </row>
-    <row r="119" spans="1:20" ht="16">
+    <row r="119" spans="1:20" ht="15.6" hidden="1">
       <c r="A119" s="7" t="s">
         <v>202</v>
       </c>
@@ -4696,7 +4698,7 @@
         <v>573</v>
       </c>
     </row>
-    <row r="120" spans="1:20" ht="16">
+    <row r="120" spans="1:20" ht="15.6" hidden="1">
       <c r="A120" s="7" t="s">
         <v>203</v>
       </c>
@@ -4714,7 +4716,7 @@
         <v>573</v>
       </c>
     </row>
-    <row r="121" spans="1:20" ht="16">
+    <row r="121" spans="1:20" ht="15.6" hidden="1">
       <c r="A121" s="7" t="s">
         <v>204</v>
       </c>
@@ -4732,7 +4734,7 @@
         <v>573</v>
       </c>
     </row>
-    <row r="122" spans="1:20" ht="16">
+    <row r="122" spans="1:20" ht="15.6">
       <c r="A122" s="7" t="s">
         <v>205</v>
       </c>
@@ -4750,7 +4752,7 @@
         <v>573</v>
       </c>
     </row>
-    <row r="123" spans="1:20" ht="16">
+    <row r="123" spans="1:20" ht="15.6" hidden="1">
       <c r="A123" s="7" t="s">
         <v>206</v>
       </c>
@@ -4768,7 +4770,7 @@
         <v>573</v>
       </c>
     </row>
-    <row r="124" spans="1:20" ht="16">
+    <row r="124" spans="1:20" ht="15.6" hidden="1">
       <c r="A124" s="7" t="s">
         <v>207</v>
       </c>
@@ -4786,7 +4788,7 @@
         <v>573</v>
       </c>
     </row>
-    <row r="125" spans="1:20" ht="16">
+    <row r="125" spans="1:20" ht="15.6" hidden="1">
       <c r="A125" s="7" t="s">
         <v>208</v>
       </c>
@@ -4804,7 +4806,7 @@
         <v>573</v>
       </c>
     </row>
-    <row r="126" spans="1:20" ht="16">
+    <row r="126" spans="1:20" ht="15.6" hidden="1">
       <c r="A126" s="7" t="s">
         <v>209</v>
       </c>
@@ -4822,7 +4824,7 @@
         <v>573</v>
       </c>
     </row>
-    <row r="127" spans="1:20" ht="16">
+    <row r="127" spans="1:20" ht="15.6" hidden="1">
       <c r="A127" s="7" t="s">
         <v>210</v>
       </c>
@@ -4840,7 +4842,7 @@
         <v>573</v>
       </c>
     </row>
-    <row r="128" spans="1:20" ht="16">
+    <row r="128" spans="1:20" ht="15.6" hidden="1">
       <c r="A128" s="7" t="s">
         <v>211</v>
       </c>
@@ -4858,7 +4860,7 @@
         <v>573</v>
       </c>
     </row>
-    <row r="129" spans="1:20" ht="16">
+    <row r="129" spans="1:20" ht="15.6">
       <c r="A129" s="7" t="s">
         <v>212</v>
       </c>
@@ -4876,7 +4878,7 @@
         <v>573</v>
       </c>
     </row>
-    <row r="130" spans="1:20" ht="16">
+    <row r="130" spans="1:20" ht="15.6" hidden="1">
       <c r="A130" s="7" t="s">
         <v>213</v>
       </c>
@@ -4894,7 +4896,7 @@
         <v>573</v>
       </c>
     </row>
-    <row r="131" spans="1:20" ht="16">
+    <row r="131" spans="1:20" ht="15.6" hidden="1">
       <c r="A131" s="7" t="s">
         <v>214</v>
       </c>
@@ -4912,7 +4914,7 @@
         <v>573</v>
       </c>
     </row>
-    <row r="132" spans="1:20" ht="16">
+    <row r="132" spans="1:20" ht="15.6" hidden="1">
       <c r="A132" s="7" t="s">
         <v>215</v>
       </c>
@@ -4930,7 +4932,7 @@
         <v>573</v>
       </c>
     </row>
-    <row r="133" spans="1:20" ht="16">
+    <row r="133" spans="1:20" ht="15.6" hidden="1">
       <c r="A133" s="7" t="s">
         <v>216</v>
       </c>
@@ -4948,7 +4950,7 @@
         <v>573</v>
       </c>
     </row>
-    <row r="134" spans="1:20" ht="16">
+    <row r="134" spans="1:20" ht="15.6">
       <c r="A134" s="7" t="s">
         <v>217</v>
       </c>
@@ -4966,7 +4968,7 @@
         <v>573</v>
       </c>
     </row>
-    <row r="135" spans="1:20" ht="16">
+    <row r="135" spans="1:20" ht="15.6" hidden="1">
       <c r="A135" s="7" t="s">
         <v>218</v>
       </c>
@@ -4984,7 +4986,7 @@
         <v>573</v>
       </c>
     </row>
-    <row r="136" spans="1:20" ht="16">
+    <row r="136" spans="1:20" ht="15.6" hidden="1">
       <c r="A136" s="7" t="s">
         <v>219</v>
       </c>
@@ -5002,7 +5004,7 @@
         <v>573</v>
       </c>
     </row>
-    <row r="137" spans="1:20" ht="16">
+    <row r="137" spans="1:20" ht="15.6" hidden="1">
       <c r="A137" s="7" t="s">
         <v>220</v>
       </c>
@@ -5020,7 +5022,7 @@
         <v>573</v>
       </c>
     </row>
-    <row r="138" spans="1:20" ht="16">
+    <row r="138" spans="1:20" ht="15.6">
       <c r="A138" s="7" t="s">
         <v>221</v>
       </c>
@@ -5038,7 +5040,7 @@
         <v>573</v>
       </c>
     </row>
-    <row r="139" spans="1:20" ht="16">
+    <row r="139" spans="1:20" ht="15.6" hidden="1">
       <c r="A139" s="7" t="s">
         <v>222</v>
       </c>
@@ -5056,7 +5058,7 @@
         <v>573</v>
       </c>
     </row>
-    <row r="140" spans="1:20" ht="16">
+    <row r="140" spans="1:20" ht="15.6">
       <c r="A140" s="7" t="s">
         <v>223</v>
       </c>
@@ -5074,7 +5076,7 @@
         <v>573</v>
       </c>
     </row>
-    <row r="141" spans="1:20" ht="16">
+    <row r="141" spans="1:20" ht="15.6" hidden="1">
       <c r="A141" s="7" t="s">
         <v>224</v>
       </c>
@@ -5092,7 +5094,7 @@
         <v>573</v>
       </c>
     </row>
-    <row r="142" spans="1:20" ht="16">
+    <row r="142" spans="1:20" ht="15.6" hidden="1">
       <c r="A142" s="7" t="s">
         <v>225</v>
       </c>
@@ -5110,7 +5112,7 @@
         <v>573</v>
       </c>
     </row>
-    <row r="143" spans="1:20" ht="16">
+    <row r="143" spans="1:20" ht="15.6" hidden="1">
       <c r="A143" s="7" t="s">
         <v>226</v>
       </c>
@@ -5128,7 +5130,7 @@
         <v>573</v>
       </c>
     </row>
-    <row r="144" spans="1:20" ht="16">
+    <row r="144" spans="1:20" ht="15.6" hidden="1">
       <c r="A144" s="7" t="s">
         <v>227</v>
       </c>
@@ -5146,7 +5148,7 @@
         <v>573</v>
       </c>
     </row>
-    <row r="145" spans="1:20" ht="16">
+    <row r="145" spans="1:20" ht="15.6">
       <c r="A145" s="7" t="s">
         <v>228</v>
       </c>
@@ -5164,7 +5166,7 @@
         <v>573</v>
       </c>
     </row>
-    <row r="146" spans="1:20" ht="16">
+    <row r="146" spans="1:20" ht="15.6" hidden="1">
       <c r="A146" s="7" t="s">
         <v>229</v>
       </c>
@@ -5182,7 +5184,7 @@
         <v>573</v>
       </c>
     </row>
-    <row r="147" spans="1:20" ht="16">
+    <row r="147" spans="1:20" ht="15.6" hidden="1">
       <c r="A147" s="7" t="s">
         <v>230</v>
       </c>
@@ -5200,7 +5202,7 @@
         <v>573</v>
       </c>
     </row>
-    <row r="148" spans="1:20" ht="16">
+    <row r="148" spans="1:20" ht="15.6" hidden="1">
       <c r="A148" s="7" t="s">
         <v>231</v>
       </c>
@@ -5218,7 +5220,7 @@
         <v>573</v>
       </c>
     </row>
-    <row r="149" spans="1:20" ht="16">
+    <row r="149" spans="1:20" ht="15.6" hidden="1">
       <c r="A149" s="7" t="s">
         <v>232</v>
       </c>
@@ -5236,7 +5238,7 @@
         <v>573</v>
       </c>
     </row>
-    <row r="150" spans="1:20" ht="16">
+    <row r="150" spans="1:20" ht="15.6" hidden="1">
       <c r="A150" s="7" t="s">
         <v>233</v>
       </c>
@@ -5254,7 +5256,7 @@
         <v>573</v>
       </c>
     </row>
-    <row r="151" spans="1:20" ht="16">
+    <row r="151" spans="1:20" ht="15.6" hidden="1">
       <c r="A151" s="7" t="s">
         <v>234</v>
       </c>
@@ -5272,7 +5274,7 @@
         <v>573</v>
       </c>
     </row>
-    <row r="152" spans="1:20" ht="16">
+    <row r="152" spans="1:20" ht="15.6" hidden="1">
       <c r="A152" s="7" t="s">
         <v>235</v>
       </c>
@@ -5290,7 +5292,7 @@
         <v>573</v>
       </c>
     </row>
-    <row r="153" spans="1:20" ht="16">
+    <row r="153" spans="1:20" ht="15.6" hidden="1">
       <c r="A153" s="7" t="s">
         <v>236</v>
       </c>
@@ -5308,7 +5310,7 @@
         <v>573</v>
       </c>
     </row>
-    <row r="154" spans="1:20" ht="16">
+    <row r="154" spans="1:20" ht="15.6" hidden="1">
       <c r="A154" s="7" t="s">
         <v>237</v>
       </c>
@@ -5326,7 +5328,7 @@
         <v>573</v>
       </c>
     </row>
-    <row r="155" spans="1:20" ht="16">
+    <row r="155" spans="1:20" ht="15.6" hidden="1">
       <c r="A155" s="7" t="s">
         <v>238</v>
       </c>
@@ -5344,7 +5346,7 @@
         <v>573</v>
       </c>
     </row>
-    <row r="156" spans="1:20" ht="16">
+    <row r="156" spans="1:20" ht="15.6" hidden="1">
       <c r="A156" s="7" t="s">
         <v>239</v>
       </c>
@@ -5362,7 +5364,7 @@
         <v>573</v>
       </c>
     </row>
-    <row r="157" spans="1:20" ht="16">
+    <row r="157" spans="1:20" ht="15.6" hidden="1">
       <c r="A157" s="7" t="s">
         <v>240</v>
       </c>
@@ -5380,7 +5382,7 @@
         <v>573</v>
       </c>
     </row>
-    <row r="158" spans="1:20" ht="16">
+    <row r="158" spans="1:20" ht="15.6">
       <c r="A158" s="7" t="s">
         <v>241</v>
       </c>
@@ -5398,7 +5400,7 @@
         <v>573</v>
       </c>
     </row>
-    <row r="159" spans="1:20" ht="16">
+    <row r="159" spans="1:20" ht="15.6" hidden="1">
       <c r="A159" s="7" t="s">
         <v>242</v>
       </c>
@@ -5416,7 +5418,7 @@
         <v>573</v>
       </c>
     </row>
-    <row r="160" spans="1:20" ht="16">
+    <row r="160" spans="1:20" ht="15.6" hidden="1">
       <c r="A160" s="7" t="s">
         <v>243</v>
       </c>
@@ -5434,7 +5436,7 @@
         <v>573</v>
       </c>
     </row>
-    <row r="161" spans="1:20" ht="16">
+    <row r="161" spans="1:20" ht="15.6" hidden="1">
       <c r="A161" s="7" t="s">
         <v>244</v>
       </c>
@@ -5452,7 +5454,7 @@
         <v>573</v>
       </c>
     </row>
-    <row r="162" spans="1:20" ht="16">
+    <row r="162" spans="1:20" ht="15.6" hidden="1">
       <c r="A162" s="7" t="s">
         <v>245</v>
       </c>
@@ -5470,7 +5472,7 @@
         <v>573</v>
       </c>
     </row>
-    <row r="163" spans="1:20" ht="16">
+    <row r="163" spans="1:20" ht="15.6" hidden="1">
       <c r="A163" s="7" t="s">
         <v>246</v>
       </c>
@@ -5488,7 +5490,7 @@
         <v>573</v>
       </c>
     </row>
-    <row r="164" spans="1:20" ht="16">
+    <row r="164" spans="1:20" ht="15.6" hidden="1">
       <c r="A164" s="7" t="s">
         <v>247</v>
       </c>
@@ -5506,7 +5508,7 @@
         <v>573</v>
       </c>
     </row>
-    <row r="165" spans="1:20" ht="16">
+    <row r="165" spans="1:20" ht="15.6">
       <c r="A165" s="7" t="s">
         <v>248</v>
       </c>
@@ -5517,14 +5519,14 @@
         <v>2019</v>
       </c>
       <c r="E165" t="s">
-        <v>572</v>
+        <v>575</v>
       </c>
       <c r="S165" s="6"/>
       <c r="T165" s="27" t="s">
         <v>573</v>
       </c>
     </row>
-    <row r="166" spans="1:20" ht="16">
+    <row r="166" spans="1:20" ht="15.6" hidden="1">
       <c r="A166" s="7" t="s">
         <v>249</v>
       </c>
@@ -5542,7 +5544,7 @@
         <v>573</v>
       </c>
     </row>
-    <row r="167" spans="1:20" ht="16">
+    <row r="167" spans="1:20" ht="15.6" hidden="1">
       <c r="A167" s="7" t="s">
         <v>250</v>
       </c>
@@ -5560,7 +5562,7 @@
         <v>573</v>
       </c>
     </row>
-    <row r="168" spans="1:20" ht="16">
+    <row r="168" spans="1:20" ht="15.6" hidden="1">
       <c r="A168" s="7" t="s">
         <v>251</v>
       </c>
@@ -5578,7 +5580,7 @@
         <v>573</v>
       </c>
     </row>
-    <row r="169" spans="1:20" ht="16">
+    <row r="169" spans="1:20" ht="15.6" hidden="1">
       <c r="A169" s="7" t="s">
         <v>252</v>
       </c>
@@ -5596,7 +5598,7 @@
         <v>573</v>
       </c>
     </row>
-    <row r="170" spans="1:20" ht="16">
+    <row r="170" spans="1:20" ht="15.6" hidden="1">
       <c r="A170" s="7" t="s">
         <v>253</v>
       </c>
@@ -5614,7 +5616,7 @@
         <v>573</v>
       </c>
     </row>
-    <row r="171" spans="1:20" ht="16">
+    <row r="171" spans="1:20" ht="15.6" hidden="1">
       <c r="A171" s="7" t="s">
         <v>254</v>
       </c>
@@ -5632,7 +5634,7 @@
         <v>573</v>
       </c>
     </row>
-    <row r="172" spans="1:20" ht="16">
+    <row r="172" spans="1:20" ht="15.6" hidden="1">
       <c r="A172" s="7" t="s">
         <v>255</v>
       </c>
@@ -5650,7 +5652,7 @@
         <v>573</v>
       </c>
     </row>
-    <row r="173" spans="1:20" ht="16">
+    <row r="173" spans="1:20" ht="15.6" hidden="1">
       <c r="A173" s="7" t="s">
         <v>256</v>
       </c>
@@ -5668,7 +5670,7 @@
         <v>573</v>
       </c>
     </row>
-    <row r="174" spans="1:20" ht="16">
+    <row r="174" spans="1:20" ht="15.6">
       <c r="A174" s="7" t="s">
         <v>257</v>
       </c>
@@ -5686,7 +5688,7 @@
         <v>573</v>
       </c>
     </row>
-    <row r="175" spans="1:20" ht="16">
+    <row r="175" spans="1:20" ht="15.6" hidden="1">
       <c r="A175" s="7" t="s">
         <v>258</v>
       </c>
@@ -5704,7 +5706,7 @@
         <v>573</v>
       </c>
     </row>
-    <row r="176" spans="1:20" ht="16">
+    <row r="176" spans="1:20" ht="15.6">
       <c r="A176" s="7" t="s">
         <v>259</v>
       </c>
@@ -5722,7 +5724,7 @@
         <v>573</v>
       </c>
     </row>
-    <row r="177" spans="1:20" ht="16">
+    <row r="177" spans="1:20" ht="15.6" hidden="1">
       <c r="A177" s="7" t="s">
         <v>260</v>
       </c>
@@ -5740,7 +5742,7 @@
         <v>573</v>
       </c>
     </row>
-    <row r="178" spans="1:20" ht="16">
+    <row r="178" spans="1:20" ht="15.6" hidden="1">
       <c r="A178" s="7" t="s">
         <v>261</v>
       </c>
@@ -5758,7 +5760,7 @@
         <v>573</v>
       </c>
     </row>
-    <row r="179" spans="1:20" ht="16">
+    <row r="179" spans="1:20" ht="15.6" hidden="1">
       <c r="A179" s="7" t="s">
         <v>262</v>
       </c>
@@ -5776,7 +5778,7 @@
         <v>573</v>
       </c>
     </row>
-    <row r="180" spans="1:20" ht="16">
+    <row r="180" spans="1:20" ht="15.6" hidden="1">
       <c r="A180" s="7" t="s">
         <v>263</v>
       </c>
@@ -5794,7 +5796,7 @@
         <v>573</v>
       </c>
     </row>
-    <row r="181" spans="1:20" ht="16">
+    <row r="181" spans="1:20" ht="15.6" hidden="1">
       <c r="A181" s="7" t="s">
         <v>264</v>
       </c>
@@ -5812,7 +5814,7 @@
         <v>573</v>
       </c>
     </row>
-    <row r="182" spans="1:20" ht="16">
+    <row r="182" spans="1:20" ht="15.6" hidden="1">
       <c r="A182" s="7" t="s">
         <v>265</v>
       </c>
@@ -5830,7 +5832,7 @@
         <v>573</v>
       </c>
     </row>
-    <row r="183" spans="1:20" ht="16">
+    <row r="183" spans="1:20" ht="15.6" hidden="1">
       <c r="A183" s="7" t="s">
         <v>266</v>
       </c>
@@ -5848,7 +5850,7 @@
         <v>573</v>
       </c>
     </row>
-    <row r="184" spans="1:20" ht="16">
+    <row r="184" spans="1:20" ht="15.6">
       <c r="A184" s="7" t="s">
         <v>267</v>
       </c>
@@ -5866,7 +5868,7 @@
         <v>573</v>
       </c>
     </row>
-    <row r="185" spans="1:20" ht="16">
+    <row r="185" spans="1:20" ht="15.6" hidden="1">
       <c r="A185" s="7" t="s">
         <v>268</v>
       </c>
@@ -5884,7 +5886,7 @@
         <v>573</v>
       </c>
     </row>
-    <row r="186" spans="1:20" ht="16">
+    <row r="186" spans="1:20" ht="15.6" hidden="1">
       <c r="A186" s="7" t="s">
         <v>269</v>
       </c>
@@ -5902,7 +5904,7 @@
         <v>573</v>
       </c>
     </row>
-    <row r="187" spans="1:20" ht="16">
+    <row r="187" spans="1:20" ht="15.6" hidden="1">
       <c r="A187" s="7" t="s">
         <v>270</v>
       </c>
@@ -5920,7 +5922,7 @@
         <v>573</v>
       </c>
     </row>
-    <row r="188" spans="1:20" ht="16">
+    <row r="188" spans="1:20" ht="15.6" hidden="1">
       <c r="A188" s="7" t="s">
         <v>271</v>
       </c>
@@ -5938,7 +5940,7 @@
         <v>573</v>
       </c>
     </row>
-    <row r="189" spans="1:20" ht="16">
+    <row r="189" spans="1:20" ht="15.6" hidden="1">
       <c r="A189" s="7" t="s">
         <v>272</v>
       </c>
@@ -5956,7 +5958,7 @@
         <v>573</v>
       </c>
     </row>
-    <row r="190" spans="1:20" ht="16">
+    <row r="190" spans="1:20" ht="15.6" hidden="1">
       <c r="A190" s="7" t="s">
         <v>273</v>
       </c>
@@ -5974,7 +5976,7 @@
         <v>573</v>
       </c>
     </row>
-    <row r="191" spans="1:20" ht="16">
+    <row r="191" spans="1:20" ht="15.6" hidden="1">
       <c r="A191" s="7" t="s">
         <v>274</v>
       </c>
@@ -5992,7 +5994,7 @@
         <v>573</v>
       </c>
     </row>
-    <row r="192" spans="1:20" ht="16">
+    <row r="192" spans="1:20" ht="15.6" hidden="1">
       <c r="A192" s="7" t="s">
         <v>275</v>
       </c>
@@ -6010,7 +6012,7 @@
         <v>573</v>
       </c>
     </row>
-    <row r="193" spans="1:20" ht="16">
+    <row r="193" spans="1:20" ht="15.6" hidden="1">
       <c r="A193" s="7" t="s">
         <v>276</v>
       </c>
@@ -6028,7 +6030,7 @@
         <v>573</v>
       </c>
     </row>
-    <row r="194" spans="1:20" ht="16">
+    <row r="194" spans="1:20" ht="15.6" hidden="1">
       <c r="A194" s="7" t="s">
         <v>277</v>
       </c>
@@ -6046,7 +6048,7 @@
         <v>573</v>
       </c>
     </row>
-    <row r="195" spans="1:20" ht="16">
+    <row r="195" spans="1:20" ht="15.6" hidden="1">
       <c r="A195" s="7" t="s">
         <v>278</v>
       </c>
@@ -6064,7 +6066,7 @@
         <v>573</v>
       </c>
     </row>
-    <row r="196" spans="1:20" ht="16">
+    <row r="196" spans="1:20" ht="15.6" hidden="1">
       <c r="A196" s="7" t="s">
         <v>279</v>
       </c>
@@ -6082,6 +6084,14 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:AJ196" xr:uid="{486982E3-56F7-4868-8DD5-43B9883CA8DC}">
+    <filterColumn colId="4">
+      <filters>
+        <filter val="Countries where national laws fully address community land tenure"/>
+        <filter val="Countries where national laws fully address community land tenure:"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -6095,21 +6105,21 @@
       <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="15.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.83203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.77734375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="21.1640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.44140625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.1640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="16.83203125" customWidth="1"/>
-    <col min="11" max="11" width="21.1640625" customWidth="1"/>
-    <col min="18" max="18" width="20.1640625" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="89.1640625" customWidth="1"/>
-    <col min="20" max="20" width="33.5" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="27.5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.77734375" customWidth="1"/>
+    <col min="11" max="11" width="21.109375" customWidth="1"/>
+    <col min="18" max="18" width="20.109375" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="89.109375" customWidth="1"/>
+    <col min="20" max="20" width="33.44140625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="27.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:24">
@@ -13685,11 +13695,11 @@
       <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="40.1640625" customWidth="1"/>
-    <col min="2" max="2" width="26.1640625" customWidth="1"/>
-    <col min="3" max="3" width="35.83203125" customWidth="1"/>
+    <col min="1" max="1" width="40.109375" customWidth="1"/>
+    <col min="2" max="2" width="26.109375" customWidth="1"/>
+    <col min="3" max="3" width="35.77734375" customWidth="1"/>
     <col min="4" max="4" width="35" customWidth="1"/>
   </cols>
   <sheetData>
@@ -14184,21 +14194,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD6C7E77-FF0A-E84A-99FE-DC85AB833D10}">
   <dimension ref="A1:G229"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
+    <sheetView zoomScale="150" workbookViewId="0">
       <selection activeCell="B1" sqref="B1:C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4"/>
   <cols>
     <col min="2" max="2" width="40" style="14" customWidth="1"/>
-    <col min="3" max="3" width="21.5" style="12" customWidth="1"/>
-    <col min="4" max="4" width="22.1640625" style="12" customWidth="1"/>
-    <col min="5" max="5" width="27.1640625" style="13" customWidth="1"/>
-    <col min="6" max="6" width="78.5" style="14" customWidth="1"/>
-    <col min="7" max="7" width="10.83203125" style="14"/>
+    <col min="3" max="3" width="21.44140625" style="12" customWidth="1"/>
+    <col min="4" max="4" width="22.109375" style="12" customWidth="1"/>
+    <col min="5" max="5" width="27.109375" style="13" customWidth="1"/>
+    <col min="6" max="6" width="78.44140625" style="14" customWidth="1"/>
+    <col min="7" max="7" width="10.77734375" style="14"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="16">
+    <row r="1" spans="1:6" ht="28.8">
       <c r="A1" s="1"/>
       <c r="B1" s="11" t="s">
         <v>568</v>
@@ -14207,7 +14217,7 @@
         <v>567</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="84">
+    <row r="2" spans="1:6" ht="71.400000000000006">
       <c r="B2" s="24" t="s">
         <v>564</v>
       </c>
@@ -14216,7 +14226,7 @@
         <v>573</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="45">
+    <row r="3" spans="1:6" ht="55.2">
       <c r="C3" s="22"/>
       <c r="D3" s="22"/>
       <c r="E3" s="23" t="s">
@@ -14357,7 +14367,7 @@
         <v>565</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="16">
+    <row r="15" spans="1:6" ht="15.6">
       <c r="C15" s="16" t="s">
         <v>377</v>
       </c>
@@ -14707,7 +14717,7 @@
         <v>574</v>
       </c>
     </row>
-    <row r="40" spans="3:6" ht="16">
+    <row r="40" spans="3:6" ht="15.6">
       <c r="C40" s="16" t="s">
         <v>402</v>
       </c>
@@ -15015,7 +15025,7 @@
         <v>565</v>
       </c>
     </row>
-    <row r="62" spans="3:6" ht="16">
+    <row r="62" spans="3:6" ht="15.6">
       <c r="C62" s="16" t="s">
         <v>424</v>
       </c>
@@ -15057,7 +15067,7 @@
         <v>565</v>
       </c>
     </row>
-    <row r="65" spans="3:6" ht="16">
+    <row r="65" spans="3:6" ht="15.6">
       <c r="C65" s="16" t="s">
         <v>427</v>
       </c>
@@ -15099,7 +15109,7 @@
         <v>574</v>
       </c>
     </row>
-    <row r="68" spans="3:6" ht="16">
+    <row r="68" spans="3:6" ht="15.6">
       <c r="C68" s="16" t="s">
         <v>430</v>
       </c>
@@ -15127,7 +15137,7 @@
         <v>565</v>
       </c>
     </row>
-    <row r="70" spans="3:6" ht="16">
+    <row r="70" spans="3:6" ht="15.6">
       <c r="C70" s="16" t="s">
         <v>432</v>
       </c>
@@ -15295,7 +15305,7 @@
         <v>571</v>
       </c>
     </row>
-    <row r="82" spans="3:6" ht="16">
+    <row r="82" spans="3:6" ht="15.6">
       <c r="C82" s="16" t="s">
         <v>444</v>
       </c>
@@ -15309,7 +15319,7 @@
         <v>570</v>
       </c>
     </row>
-    <row r="83" spans="3:6" ht="16">
+    <row r="83" spans="3:6" ht="15.6">
       <c r="C83" s="16" t="s">
         <v>445</v>
       </c>
@@ -15589,7 +15599,7 @@
         <v>565</v>
       </c>
     </row>
-    <row r="103" spans="3:6" ht="16">
+    <row r="103" spans="3:6" ht="15.6">
       <c r="C103" s="16" t="s">
         <v>466</v>
       </c>
@@ -15813,7 +15823,7 @@
         <v>565</v>
       </c>
     </row>
-    <row r="119" spans="3:6" ht="16">
+    <row r="119" spans="3:6" ht="15.6">
       <c r="C119" s="16" t="s">
         <v>482</v>
       </c>
@@ -16037,7 +16047,7 @@
         <v>565</v>
       </c>
     </row>
-    <row r="135" spans="3:6" ht="16">
+    <row r="135" spans="3:6" ht="15.6">
       <c r="C135" s="16" t="s">
         <v>498</v>
       </c>
@@ -16205,7 +16215,7 @@
         <v>574</v>
       </c>
     </row>
-    <row r="147" spans="3:6" ht="16">
+    <row r="147" spans="3:6" ht="15.6">
       <c r="C147" s="16" t="s">
         <v>510</v>
       </c>
@@ -16443,7 +16453,7 @@
         <v>565</v>
       </c>
     </row>
-    <row r="164" spans="2:6" ht="16">
+    <row r="164" spans="2:6" ht="15.6">
       <c r="C164" s="16" t="s">
         <v>527</v>
       </c>
@@ -16499,7 +16509,7 @@
         <v>565</v>
       </c>
     </row>
-    <row r="168" spans="2:6" ht="16">
+    <row r="168" spans="2:6" ht="15.6">
       <c r="C168" s="16" t="s">
         <v>531</v>
       </c>
@@ -16795,7 +16805,7 @@
         <v>575</v>
       </c>
     </row>
-    <row r="189" spans="2:6" ht="16">
+    <row r="189" spans="2:6" ht="15.6">
       <c r="C189" s="16" t="s">
         <v>552</v>
       </c>
@@ -16907,7 +16917,7 @@
         <v>565</v>
       </c>
     </row>
-    <row r="197" spans="3:6" ht="16">
+    <row r="197" spans="3:6" ht="15.6">
       <c r="C197" s="16" t="s">
         <v>560</v>
       </c>
@@ -16935,7 +16945,7 @@
         <v>574</v>
       </c>
     </row>
-    <row r="199" spans="3:6" ht="16">
+    <row r="199" spans="3:6" ht="15.6">
       <c r="C199" s="16" t="s">
         <v>562</v>
       </c>
@@ -16991,9 +17001,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -17169,26 +17182,15 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{44D4A413-FCE6-452E-998A-26A273C51DAD}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6962EFDB-3713-4253-9AC6-1F6EE91D9C4E}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="48b2e3f7-b09f-47ae-8574-fd5d5ffa6be8"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -17212,9 +17214,17 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6962EFDB-3713-4253-9AC6-1F6EE91D9C4E}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{44D4A413-FCE6-452E-998A-26A273C51DAD}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="48b2e3f7-b09f-47ae-8574-fd5d5ffa6be8"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>